<commit_message>
The end? Finished examples
</commit_message>
<xml_diff>
--- a/Arkusze/Doktorat_obliczenia_EU-28_mediana.xlsx
+++ b/Arkusze/Doktorat_obliczenia_EU-28_mediana.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zemat\OneDrive\R_Map_Stats_GreenJobs\Arkusze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="102_{665F6A43-D7A3-42E6-9044-C8679C03ED13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{41FF2A7B-45FD-4561-8AD5-43CC6B89F0E8}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="102_{665F6A43-D7A3-42E6-9044-C8679C03ED13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{E765A357-7EA0-4DBA-8AC3-4C8B597EE39D}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="60" windowWidth="15195" windowHeight="9210" tabRatio="952" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39701,7 +39701,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -58724,7 +58724,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -58735,7 +58735,15 @@
     <col min="8" max="11" width="9.140625" style="6"/>
     <col min="12" max="12" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="9.140625" style="6"/>
-    <col min="17" max="25" width="9.140625" style="7"/>
+    <col min="17" max="17" width="9.140625" style="7"/>
+    <col min="18" max="18" width="31.85546875" style="7" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="7"/>
+    <col min="20" max="20" width="17.140625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="7"/>
+    <col min="22" max="22" width="15" style="7" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" style="7"/>
+    <col min="24" max="24" width="23.28515625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="7"/>
     <col min="26" max="27" width="9.140625" style="6"/>
     <col min="28" max="28" width="9.140625" style="7"/>
     <col min="29" max="29" width="9.7109375" style="7" bestFit="1" customWidth="1"/>
@@ -58963,19 +58971,19 @@
         <v>169.6</v>
       </c>
       <c r="AC2" s="10">
-        <f>((B2-$B$30)^2+(C2-$C$30)^2+(D2-$D$30)^2+(E2-$E$30)^2+(F2-$F$30)^2+(G2-$G$30)^2+(H2-$H$30)^2+(I2-$I$30)^2+(J2-$J$30)^2+(K2-$K$30)^2+(L2-$L$30)^2+(M2-$M$30)^2+(N2-$N$30)^2+(O2-$O$30)^2+(P2-$P$30)^2+(Q2-$Q$30)^2+(R2-$R$30)^2+(S2-$S$30)^2+(T2-$T$30)^2+(U2-$U$30)^2+(V2-$V$30)^2+(W2-$W$30)^2+(X2-$X$30)^2+(Y2-$Y$30)^2+(Z2-$Z$30)^2+(AA2-$AA$30)^2+(AB2-$AB$30)^2)^(0.5)</f>
+        <f t="shared" ref="AC2:AC29" si="0">((B2-$B$30)^2+(C2-$C$30)^2+(D2-$D$30)^2+(E2-$E$30)^2+(F2-$F$30)^2+(G2-$G$30)^2+(H2-$H$30)^2+(I2-$I$30)^2+(J2-$J$30)^2+(K2-$K$30)^2+(L2-$L$30)^2+(M2-$M$30)^2+(N2-$N$30)^2+(O2-$O$30)^2+(P2-$P$30)^2+(Q2-$Q$30)^2+(R2-$R$30)^2+(S2-$S$30)^2+(T2-$T$30)^2+(U2-$U$30)^2+(V2-$V$30)^2+(W2-$W$30)^2+(X2-$X$30)^2+(Y2-$Y$30)^2+(Z2-$Z$30)^2+(AA2-$AA$30)^2+(AB2-$AB$30)^2)^(0.5)</f>
         <v>14764.607277474399</v>
       </c>
       <c r="AD2" s="10">
-        <f>1-(AC2/$AI$2)</f>
+        <f t="shared" ref="AD2:AD29" si="1">1-(AC2/$AI$2)</f>
         <v>0.32509732118001555</v>
       </c>
       <c r="AE2" s="7" t="str">
-        <f>A2</f>
+        <f t="shared" ref="AE2:AE29" si="2">A2</f>
         <v>Austria</v>
       </c>
       <c r="AF2" s="11">
-        <f>AD2</f>
+        <f t="shared" ref="AF2:AF29" si="3">AD2</f>
         <v>0.32509732118001555</v>
       </c>
       <c r="AG2" s="11">
@@ -59105,19 +59113,19 @@
         <v>83.65</v>
       </c>
       <c r="AC3" s="10">
-        <f>((B3-$B$30)^2+(C3-$C$30)^2+(D3-$D$30)^2+(E3-$E$30)^2+(F3-$F$30)^2+(G3-$G$30)^2+(H3-$H$30)^2+(I3-$I$30)^2+(J3-$J$30)^2+(K3-$K$30)^2+(L3-$L$30)^2+(M3-$M$30)^2+(N3-$N$30)^2+(O3-$O$30)^2+(P3-$P$30)^2+(Q3-$Q$30)^2+(R3-$R$30)^2+(S3-$S$30)^2+(T3-$T$30)^2+(U3-$U$30)^2+(V3-$V$30)^2+(W3-$W$30)^2+(X3-$X$30)^2+(Y3-$Y$30)^2+(Z3-$Z$30)^2+(AA3-$AA$30)^2+(AB3-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>14474.510647603947</v>
       </c>
       <c r="AD3" s="10">
-        <f>1-(AC3/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.33835788334308226</v>
       </c>
       <c r="AE3" s="7" t="str">
-        <f>A3</f>
+        <f t="shared" si="2"/>
         <v>Belgia</v>
       </c>
       <c r="AF3" s="11">
-        <f>AD3</f>
+        <f t="shared" si="3"/>
         <v>0.33835788334308226</v>
       </c>
       <c r="AG3" s="11">
@@ -59246,19 +59254,19 @@
         <v>32</v>
       </c>
       <c r="AC4" s="10">
-        <f>((B4-$B$30)^2+(C4-$C$30)^2+(D4-$D$30)^2+(E4-$E$30)^2+(F4-$F$30)^2+(G4-$G$30)^2+(H4-$H$30)^2+(I4-$I$30)^2+(J4-$J$30)^2+(K4-$K$30)^2+(L4-$L$30)^2+(M4-$M$30)^2+(N4-$N$30)^2+(O4-$O$30)^2+(P4-$P$30)^2+(Q4-$Q$30)^2+(R4-$R$30)^2+(S4-$S$30)^2+(T4-$T$30)^2+(U4-$U$30)^2+(V4-$V$30)^2+(W4-$W$30)^2+(X4-$X$30)^2+(Y4-$Y$30)^2+(Z4-$Z$30)^2+(AA4-$AA$30)^2+(AB4-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18522.685103174161</v>
       </c>
       <c r="AD4" s="10">
-        <f>1-(AC4/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.15331240715468208</v>
       </c>
       <c r="AE4" s="7" t="str">
-        <f>A4</f>
+        <f t="shared" si="2"/>
         <v>Bułgaria</v>
       </c>
       <c r="AF4" s="11">
-        <f>AD4</f>
+        <f t="shared" si="3"/>
         <v>0.15331240715468208</v>
       </c>
       <c r="AG4" s="7" t="s">
@@ -59385,19 +59393,19 @@
         <v>48.1</v>
       </c>
       <c r="AC5" s="10">
-        <f>((B5-$B$30)^2+(C5-$C$30)^2+(D5-$D$30)^2+(E5-$E$30)^2+(F5-$F$30)^2+(G5-$G$30)^2+(H5-$H$30)^2+(I5-$I$30)^2+(J5-$J$30)^2+(K5-$K$30)^2+(L5-$L$30)^2+(M5-$M$30)^2+(N5-$N$30)^2+(O5-$O$30)^2+(P5-$P$30)^2+(Q5-$Q$30)^2+(R5-$R$30)^2+(S5-$S$30)^2+(T5-$T$30)^2+(U5-$U$30)^2+(V5-$V$30)^2+(W5-$W$30)^2+(X5-$X$30)^2+(Y5-$Y$30)^2+(Z5-$Z$30)^2+(AA5-$AA$30)^2+(AB5-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>16570.543530112398</v>
       </c>
       <c r="AD5" s="10">
-        <f>1-(AC5/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.24254644855755048</v>
       </c>
       <c r="AE5" s="7" t="str">
-        <f>A5</f>
+        <f t="shared" si="2"/>
         <v>Chorwacja</v>
       </c>
       <c r="AF5" s="11">
-        <f>AD5</f>
+        <f t="shared" si="3"/>
         <v>0.24254644855755048</v>
       </c>
       <c r="AG5" s="7" t="s">
@@ -59524,19 +59532,19 @@
         <v>144.90352633826882</v>
       </c>
       <c r="AC6" s="10">
-        <f>((B6-$B$30)^2+(C6-$C$30)^2+(D6-$D$30)^2+(E6-$E$30)^2+(F6-$F$30)^2+(G6-$G$30)^2+(H6-$H$30)^2+(I6-$I$30)^2+(J6-$J$30)^2+(K6-$K$30)^2+(L6-$L$30)^2+(M6-$M$30)^2+(N6-$N$30)^2+(O6-$O$30)^2+(P6-$P$30)^2+(Q6-$Q$30)^2+(R6-$R$30)^2+(S6-$S$30)^2+(T6-$T$30)^2+(U6-$U$30)^2+(V6-$V$30)^2+(W6-$W$30)^2+(X6-$X$30)^2+(Y6-$Y$30)^2+(Z6-$Z$30)^2+(AA6-$AA$30)^2+(AB6-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>15906.383989462982</v>
       </c>
       <c r="AD6" s="10">
-        <f>1-(AC6/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.27290574255868538</v>
       </c>
       <c r="AE6" s="7" t="str">
-        <f>A6</f>
+        <f t="shared" si="2"/>
         <v>Cypr</v>
       </c>
       <c r="AF6" s="11">
-        <f>AD6</f>
+        <f t="shared" si="3"/>
         <v>0.27290574255868538</v>
       </c>
       <c r="AG6" s="7" t="s">
@@ -59663,19 +59671,19 @@
         <v>104.30000000000001</v>
       </c>
       <c r="AC7" s="10">
-        <f>((B7-$B$30)^2+(C7-$C$30)^2+(D7-$D$30)^2+(E7-$E$30)^2+(F7-$F$30)^2+(G7-$G$30)^2+(H7-$H$30)^2+(I7-$I$30)^2+(J7-$J$30)^2+(K7-$K$30)^2+(L7-$L$30)^2+(M7-$M$30)^2+(N7-$N$30)^2+(O7-$O$30)^2+(P7-$P$30)^2+(Q7-$Q$30)^2+(R7-$R$30)^2+(S7-$S$30)^2+(T7-$T$30)^2+(U7-$U$30)^2+(V7-$V$30)^2+(W7-$W$30)^2+(X7-$X$30)^2+(Y7-$Y$30)^2+(Z7-$Z$30)^2+(AA7-$AA$30)^2+(AB7-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>12933.530026749273</v>
       </c>
       <c r="AD7" s="10">
-        <f>1-(AC7/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.4087974100761228</v>
       </c>
       <c r="AE7" s="7" t="str">
-        <f>A7</f>
+        <f t="shared" si="2"/>
         <v>Czechy</v>
       </c>
       <c r="AF7" s="11">
-        <f>AD7</f>
+        <f t="shared" si="3"/>
         <v>0.4087974100761228</v>
       </c>
       <c r="AG7" s="7" t="s">
@@ -59802,19 +59810,19 @@
         <v>66.7</v>
       </c>
       <c r="AC8" s="10">
-        <f>((B8-$B$30)^2+(C8-$C$30)^2+(D8-$D$30)^2+(E8-$E$30)^2+(F8-$F$30)^2+(G8-$G$30)^2+(H8-$H$30)^2+(I8-$I$30)^2+(J8-$J$30)^2+(K8-$K$30)^2+(L8-$L$30)^2+(M8-$M$30)^2+(N8-$N$30)^2+(O8-$O$30)^2+(P8-$P$30)^2+(Q8-$Q$30)^2+(R8-$R$30)^2+(S8-$S$30)^2+(T8-$T$30)^2+(U8-$U$30)^2+(V8-$V$30)^2+(W8-$W$30)^2+(X8-$X$30)^2+(Y8-$Y$30)^2+(Z8-$Z$30)^2+(AA8-$AA$30)^2+(AB8-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>10447.651092530325</v>
       </c>
       <c r="AD8" s="10">
-        <f>1-(AC8/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.52242903741281177</v>
       </c>
       <c r="AE8" s="7" t="str">
-        <f>A8</f>
+        <f t="shared" si="2"/>
         <v>Dania</v>
       </c>
       <c r="AF8" s="11">
-        <f>AD8</f>
+        <f t="shared" si="3"/>
         <v>0.52242903741281177</v>
       </c>
       <c r="AG8" s="7" t="s">
@@ -59941,19 +59949,19 @@
         <v>28.25</v>
       </c>
       <c r="AC9" s="10">
-        <f>((B9-$B$30)^2+(C9-$C$30)^2+(D9-$D$30)^2+(E9-$E$30)^2+(F9-$F$30)^2+(G9-$G$30)^2+(H9-$H$30)^2+(I9-$I$30)^2+(J9-$J$30)^2+(K9-$K$30)^2+(L9-$L$30)^2+(M9-$M$30)^2+(N9-$N$30)^2+(O9-$O$30)^2+(P9-$P$30)^2+(Q9-$Q$30)^2+(R9-$R$30)^2+(S9-$S$30)^2+(T9-$T$30)^2+(U9-$U$30)^2+(V9-$V$30)^2+(W9-$W$30)^2+(X9-$X$30)^2+(Y9-$Y$30)^2+(Z9-$Z$30)^2+(AA9-$AA$30)^2+(AB9-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>16769.417946074482</v>
       </c>
       <c r="AD9" s="10">
-        <f>1-(AC9/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.23345573090017369</v>
       </c>
       <c r="AE9" s="7" t="str">
-        <f>A9</f>
+        <f t="shared" si="2"/>
         <v>Estonia</v>
       </c>
       <c r="AF9" s="11">
-        <f>AD9</f>
+        <f t="shared" si="3"/>
         <v>0.23345573090017369</v>
       </c>
       <c r="AG9" s="7" t="s">
@@ -60080,19 +60088,19 @@
         <v>132.69999999999999</v>
       </c>
       <c r="AC10" s="10">
-        <f>((B10-$B$30)^2+(C10-$C$30)^2+(D10-$D$30)^2+(E10-$E$30)^2+(F10-$F$30)^2+(G10-$G$30)^2+(H10-$H$30)^2+(I10-$I$30)^2+(J10-$J$30)^2+(K10-$K$30)^2+(L10-$L$30)^2+(M10-$M$30)^2+(N10-$N$30)^2+(O10-$O$30)^2+(P10-$P$30)^2+(Q10-$Q$30)^2+(R10-$R$30)^2+(S10-$S$30)^2+(T10-$T$30)^2+(U10-$U$30)^2+(V10-$V$30)^2+(W10-$W$30)^2+(X10-$X$30)^2+(Y10-$Y$30)^2+(Z10-$Z$30)^2+(AA10-$AA$30)^2+(AB10-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>17159.649463789319</v>
       </c>
       <c r="AD10" s="10">
-        <f>1-(AC10/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.21561791837213307</v>
       </c>
       <c r="AE10" s="7" t="str">
-        <f>A10</f>
+        <f t="shared" si="2"/>
         <v>Finlandia</v>
       </c>
       <c r="AF10" s="11">
-        <f>AD10</f>
+        <f t="shared" si="3"/>
         <v>0.21561791837213307</v>
       </c>
       <c r="AG10" s="7" t="s">
@@ -60219,19 +60227,19 @@
         <v>441.65</v>
       </c>
       <c r="AC11" s="10">
-        <f>((B11-$B$30)^2+(C11-$C$30)^2+(D11-$D$30)^2+(E11-$E$30)^2+(F11-$F$30)^2+(G11-$G$30)^2+(H11-$H$30)^2+(I11-$I$30)^2+(J11-$J$30)^2+(K11-$K$30)^2+(L11-$L$30)^2+(M11-$M$30)^2+(N11-$N$30)^2+(O11-$O$30)^2+(P11-$P$30)^2+(Q11-$Q$30)^2+(R11-$R$30)^2+(S11-$S$30)^2+(T11-$T$30)^2+(U11-$U$30)^2+(V11-$V$30)^2+(W11-$W$30)^2+(X11-$X$30)^2+(Y11-$Y$30)^2+(Z11-$Z$30)^2+(AA11-$AA$30)^2+(AB11-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>16399.212374255203</v>
       </c>
       <c r="AD11" s="10">
-        <f>1-(AC11/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.25037814051387897</v>
       </c>
       <c r="AE11" s="7" t="str">
-        <f>A11</f>
+        <f t="shared" si="2"/>
         <v>Francja</v>
       </c>
       <c r="AF11" s="11">
-        <f>AD11</f>
+        <f t="shared" si="3"/>
         <v>0.25037814051387897</v>
       </c>
       <c r="AG11" s="7" t="s">
@@ -60358,19 +60366,19 @@
         <v>145.53229055046864</v>
       </c>
       <c r="AC12" s="10">
-        <f>((B12-$B$30)^2+(C12-$C$30)^2+(D12-$D$30)^2+(E12-$E$30)^2+(F12-$F$30)^2+(G12-$G$30)^2+(H12-$H$30)^2+(I12-$I$30)^2+(J12-$J$30)^2+(K12-$K$30)^2+(L12-$L$30)^2+(M12-$M$30)^2+(N12-$N$30)^2+(O12-$O$30)^2+(P12-$P$30)^2+(Q12-$Q$30)^2+(R12-$R$30)^2+(S12-$S$30)^2+(T12-$T$30)^2+(U12-$U$30)^2+(V12-$V$30)^2+(W12-$W$30)^2+(X12-$X$30)^2+(Y12-$Y$30)^2+(Z12-$Z$30)^2+(AA12-$AA$30)^2+(AB12-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>13329.093776487227</v>
       </c>
       <c r="AD12" s="10">
-        <f>1-(AC12/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.39071585671509834</v>
       </c>
       <c r="AE12" s="7" t="str">
-        <f>A12</f>
+        <f t="shared" si="2"/>
         <v>Grecja</v>
       </c>
       <c r="AF12" s="11">
-        <f>AD12</f>
+        <f t="shared" si="3"/>
         <v>0.39071585671509834</v>
       </c>
       <c r="AG12" s="7" t="s">
@@ -60497,19 +60505,19 @@
         <v>259.75</v>
       </c>
       <c r="AC13" s="10">
-        <f>((B13-$B$30)^2+(C13-$C$30)^2+(D13-$D$30)^2+(E13-$E$30)^2+(F13-$F$30)^2+(G13-$G$30)^2+(H13-$H$30)^2+(I13-$I$30)^2+(J13-$J$30)^2+(K13-$K$30)^2+(L13-$L$30)^2+(M13-$M$30)^2+(N13-$N$30)^2+(O13-$O$30)^2+(P13-$P$30)^2+(Q13-$Q$30)^2+(R13-$R$30)^2+(S13-$S$30)^2+(T13-$T$30)^2+(U13-$U$30)^2+(V13-$V$30)^2+(W13-$W$30)^2+(X13-$X$30)^2+(Y13-$Y$30)^2+(Z13-$Z$30)^2+(AA13-$AA$30)^2+(AB13-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18366.290644590568</v>
       </c>
       <c r="AD13" s="10">
-        <f>1-(AC13/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.160461330053004</v>
       </c>
       <c r="AE13" s="7" t="str">
-        <f>A13</f>
+        <f t="shared" si="2"/>
         <v>Hiszpania</v>
       </c>
       <c r="AF13" s="11">
-        <f>AD13</f>
+        <f t="shared" si="3"/>
         <v>0.160461330053004</v>
       </c>
       <c r="AG13" s="7" t="s">
@@ -60636,19 +60644,19 @@
         <v>130.75</v>
       </c>
       <c r="AC14" s="10">
-        <f>((B14-$B$30)^2+(C14-$C$30)^2+(D14-$D$30)^2+(E14-$E$30)^2+(F14-$F$30)^2+(G14-$G$30)^2+(H14-$H$30)^2+(I14-$I$30)^2+(J14-$J$30)^2+(K14-$K$30)^2+(L14-$L$30)^2+(M14-$M$30)^2+(N14-$N$30)^2+(O14-$O$30)^2+(P14-$P$30)^2+(Q14-$Q$30)^2+(R14-$R$30)^2+(S14-$S$30)^2+(T14-$T$30)^2+(U14-$U$30)^2+(V14-$V$30)^2+(W14-$W$30)^2+(X14-$X$30)^2+(Y14-$Y$30)^2+(Z14-$Z$30)^2+(AA14-$AA$30)^2+(AB14-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>16067.48470675793</v>
       </c>
       <c r="AD14" s="10">
-        <f>1-(AC14/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.26554169259658023</v>
       </c>
       <c r="AE14" s="7" t="str">
-        <f>A14</f>
+        <f t="shared" si="2"/>
         <v>Holandia</v>
       </c>
       <c r="AF14" s="11">
-        <f>AD14</f>
+        <f t="shared" si="3"/>
         <v>0.26554169259658023</v>
       </c>
       <c r="AG14" s="7" t="s">
@@ -60775,19 +60783,19 @@
         <v>23.3</v>
       </c>
       <c r="AC15" s="10">
-        <f>((B15-$B$30)^2+(C15-$C$30)^2+(D15-$D$30)^2+(E15-$E$30)^2+(F15-$F$30)^2+(G15-$G$30)^2+(H15-$H$30)^2+(I15-$I$30)^2+(J15-$J$30)^2+(K15-$K$30)^2+(L15-$L$30)^2+(M15-$M$30)^2+(N15-$N$30)^2+(O15-$O$30)^2+(P15-$P$30)^2+(Q15-$Q$30)^2+(R15-$R$30)^2+(S15-$S$30)^2+(T15-$T$30)^2+(U15-$U$30)^2+(V15-$V$30)^2+(W15-$W$30)^2+(X15-$X$30)^2+(Y15-$Y$30)^2+(Z15-$Z$30)^2+(AA15-$AA$30)^2+(AB15-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>17723.218691254278</v>
       </c>
       <c r="AD15" s="10">
-        <f>1-(AC15/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.18985669261322669</v>
       </c>
       <c r="AE15" s="7" t="str">
-        <f>A15</f>
+        <f t="shared" si="2"/>
         <v>Irlandia</v>
       </c>
       <c r="AF15" s="11">
-        <f>AD15</f>
+        <f t="shared" si="3"/>
         <v>0.18985669261322669</v>
       </c>
       <c r="AG15" s="7" t="s">
@@ -60914,19 +60922,19 @@
         <v>37.150000000000006</v>
       </c>
       <c r="AC16" s="10">
-        <f>((B16-$B$30)^2+(C16-$C$30)^2+(D16-$D$30)^2+(E16-$E$30)^2+(F16-$F$30)^2+(G16-$G$30)^2+(H16-$H$30)^2+(I16-$I$30)^2+(J16-$J$30)^2+(K16-$K$30)^2+(L16-$L$30)^2+(M16-$M$30)^2+(N16-$N$30)^2+(O16-$O$30)^2+(P16-$P$30)^2+(Q16-$Q$30)^2+(R16-$R$30)^2+(S16-$S$30)^2+(T16-$T$30)^2+(U16-$U$30)^2+(V16-$V$30)^2+(W16-$W$30)^2+(X16-$X$30)^2+(Y16-$Y$30)^2+(Z16-$Z$30)^2+(AA16-$AA$30)^2+(AB16-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18747.178048000314</v>
       </c>
       <c r="AD16" s="10">
-        <f>1-(AC16/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.14305064488820374</v>
       </c>
       <c r="AE16" s="7" t="str">
-        <f>A16</f>
+        <f t="shared" si="2"/>
         <v>Litwa</v>
       </c>
       <c r="AF16" s="11">
-        <f>AD16</f>
+        <f t="shared" si="3"/>
         <v>0.14305064488820374</v>
       </c>
       <c r="AG16" s="7" t="s">
@@ -61053,19 +61061,19 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="AC17" s="10">
-        <f>((B17-$B$30)^2+(C17-$C$30)^2+(D17-$D$30)^2+(E17-$E$30)^2+(F17-$F$30)^2+(G17-$G$30)^2+(H17-$H$30)^2+(I17-$I$30)^2+(J17-$J$30)^2+(K17-$K$30)^2+(L17-$L$30)^2+(M17-$M$30)^2+(N17-$N$30)^2+(O17-$O$30)^2+(P17-$P$30)^2+(Q17-$Q$30)^2+(R17-$R$30)^2+(S17-$S$30)^2+(T17-$T$30)^2+(U17-$U$30)^2+(V17-$V$30)^2+(W17-$W$30)^2+(X17-$X$30)^2+(Y17-$Y$30)^2+(Z17-$Z$30)^2+(AA17-$AA$30)^2+(AB17-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18460.475414016968</v>
       </c>
       <c r="AD17" s="10">
-        <f>1-(AC17/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.15615606463040799</v>
       </c>
       <c r="AE17" s="7" t="str">
-        <f>A17</f>
+        <f t="shared" si="2"/>
         <v>Luksemburg</v>
       </c>
       <c r="AF17" s="11">
-        <f>AD17</f>
+        <f t="shared" si="3"/>
         <v>0.15615606463040799</v>
       </c>
       <c r="AG17" s="7" t="s">
@@ -61192,19 +61200,19 @@
         <v>27.95</v>
       </c>
       <c r="AC18" s="10">
-        <f>((B18-$B$30)^2+(C18-$C$30)^2+(D18-$D$30)^2+(E18-$E$30)^2+(F18-$F$30)^2+(G18-$G$30)^2+(H18-$H$30)^2+(I18-$I$30)^2+(J18-$J$30)^2+(K18-$K$30)^2+(L18-$L$30)^2+(M18-$M$30)^2+(N18-$N$30)^2+(O18-$O$30)^2+(P18-$P$30)^2+(Q18-$Q$30)^2+(R18-$R$30)^2+(S18-$S$30)^2+(T18-$T$30)^2+(U18-$U$30)^2+(V18-$V$30)^2+(W18-$W$30)^2+(X18-$X$30)^2+(Y18-$Y$30)^2+(Z18-$Z$30)^2+(AA18-$AA$30)^2+(AB18-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>4203.9570934983385</v>
       </c>
       <c r="AD18" s="10">
-        <f>1-(AC18/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.80783356775259652</v>
       </c>
       <c r="AE18" s="7" t="str">
-        <f>A18</f>
+        <f t="shared" si="2"/>
         <v>Łotwa</v>
       </c>
       <c r="AF18" s="11">
-        <f>AD18</f>
+        <f t="shared" si="3"/>
         <v>0.80783356775259652</v>
       </c>
       <c r="AG18" s="7" t="s">
@@ -61331,19 +61339,19 @@
         <v>143.91419305977459</v>
       </c>
       <c r="AC19" s="10">
-        <f>((B19-$B$30)^2+(C19-$C$30)^2+(D19-$D$30)^2+(E19-$E$30)^2+(F19-$F$30)^2+(G19-$G$30)^2+(H19-$H$30)^2+(I19-$I$30)^2+(J19-$J$30)^2+(K19-$K$30)^2+(L19-$L$30)^2+(M19-$M$30)^2+(N19-$N$30)^2+(O19-$O$30)^2+(P19-$P$30)^2+(Q19-$Q$30)^2+(R19-$R$30)^2+(S19-$S$30)^2+(T19-$T$30)^2+(U19-$U$30)^2+(V19-$V$30)^2+(W19-$W$30)^2+(X19-$X$30)^2+(Y19-$Y$30)^2+(Z19-$Z$30)^2+(AA19-$AA$30)^2+(AB19-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18080.195670093955</v>
       </c>
       <c r="AD19" s="10">
-        <f>1-(AC19/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.17353897316642986</v>
       </c>
       <c r="AE19" s="7" t="str">
-        <f>A19</f>
+        <f t="shared" si="2"/>
         <v>Malta</v>
       </c>
       <c r="AF19" s="11">
-        <f>AD19</f>
+        <f t="shared" si="3"/>
         <v>0.17353897316642986</v>
       </c>
       <c r="AG19" s="7" t="s">
@@ -61470,19 +61478,19 @@
         <v>470.4</v>
       </c>
       <c r="AC20" s="10">
-        <f>((B20-$B$30)^2+(C20-$C$30)^2+(D20-$D$30)^2+(E20-$E$30)^2+(F20-$F$30)^2+(G20-$G$30)^2+(H20-$H$30)^2+(I20-$I$30)^2+(J20-$J$30)^2+(K20-$K$30)^2+(L20-$L$30)^2+(M20-$M$30)^2+(N20-$N$30)^2+(O20-$O$30)^2+(P20-$P$30)^2+(Q20-$Q$30)^2+(R20-$R$30)^2+(S20-$S$30)^2+(T20-$T$30)^2+(U20-$U$30)^2+(V20-$V$30)^2+(W20-$W$30)^2+(X20-$X$30)^2+(Y20-$Y$30)^2+(Z20-$Z$30)^2+(AA20-$AA$30)^2+(AB20-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18295.239542280528</v>
       </c>
       <c r="AD20" s="10">
-        <f>1-(AC20/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.16370913599738013</v>
       </c>
       <c r="AE20" s="7" t="str">
-        <f>A20</f>
+        <f t="shared" si="2"/>
         <v>Niemcy</v>
       </c>
       <c r="AF20" s="11">
-        <f>AD20</f>
+        <f t="shared" si="3"/>
         <v>0.16370913599738013</v>
       </c>
       <c r="AG20" s="7" t="s">
@@ -61609,19 +61617,19 @@
         <v>491.7</v>
       </c>
       <c r="AC21" s="10">
-        <f>((B21-$B$30)^2+(C21-$C$30)^2+(D21-$D$30)^2+(E21-$E$30)^2+(F21-$F$30)^2+(G21-$G$30)^2+(H21-$H$30)^2+(I21-$I$30)^2+(J21-$J$30)^2+(K21-$K$30)^2+(L21-$L$30)^2+(M21-$M$30)^2+(N21-$N$30)^2+(O21-$O$30)^2+(P21-$P$30)^2+(Q21-$Q$30)^2+(R21-$R$30)^2+(S21-$S$30)^2+(T21-$T$30)^2+(U21-$U$30)^2+(V21-$V$30)^2+(W21-$W$30)^2+(X21-$X$30)^2+(Y21-$Y$30)^2+(Z21-$Z$30)^2+(AA21-$AA$30)^2+(AB21-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>11672.834148757534</v>
       </c>
       <c r="AD21" s="10">
-        <f>1-(AC21/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.46642488429496165</v>
       </c>
       <c r="AE21" s="7" t="str">
-        <f>A21</f>
+        <f t="shared" si="2"/>
         <v>Polska</v>
       </c>
       <c r="AF21" s="11">
-        <f>AD21</f>
+        <f t="shared" si="3"/>
         <v>0.46642488429496165</v>
       </c>
       <c r="AG21" s="7" t="s">
@@ -61748,19 +61756,19 @@
         <v>95.699999999999989</v>
       </c>
       <c r="AC22" s="10">
-        <f>((B22-$B$30)^2+(C22-$C$30)^2+(D22-$D$30)^2+(E22-$E$30)^2+(F22-$F$30)^2+(G22-$G$30)^2+(H22-$H$30)^2+(I22-$I$30)^2+(J22-$J$30)^2+(K22-$K$30)^2+(L22-$L$30)^2+(M22-$M$30)^2+(N22-$N$30)^2+(O22-$O$30)^2+(P22-$P$30)^2+(Q22-$Q$30)^2+(R22-$R$30)^2+(S22-$S$30)^2+(T22-$T$30)^2+(U22-$U$30)^2+(V22-$V$30)^2+(W22-$W$30)^2+(X22-$X$30)^2+(Y22-$Y$30)^2+(Z22-$Z$30)^2+(AA22-$AA$30)^2+(AB22-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>14834.791985483822</v>
       </c>
       <c r="AD22" s="10">
-        <f>1-(AC22/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.32188911885146287</v>
       </c>
       <c r="AE22" s="7" t="str">
-        <f>A22</f>
+        <f t="shared" si="2"/>
         <v>Portugalia</v>
       </c>
       <c r="AF22" s="11">
-        <f>AD22</f>
+        <f t="shared" si="3"/>
         <v>0.32188911885146287</v>
       </c>
       <c r="AG22" s="7" t="s">
@@ -61887,19 +61895,19 @@
         <v>192.35</v>
       </c>
       <c r="AC23" s="10">
-        <f>((B23-$B$30)^2+(C23-$C$30)^2+(D23-$D$30)^2+(E23-$E$30)^2+(F23-$F$30)^2+(G23-$G$30)^2+(H23-$H$30)^2+(I23-$I$30)^2+(J23-$J$30)^2+(K23-$K$30)^2+(L23-$L$30)^2+(M23-$M$30)^2+(N23-$N$30)^2+(O23-$O$30)^2+(P23-$P$30)^2+(Q23-$Q$30)^2+(R23-$R$30)^2+(S23-$S$30)^2+(T23-$T$30)^2+(U23-$U$30)^2+(V23-$V$30)^2+(W23-$W$30)^2+(X23-$X$30)^2+(Y23-$Y$30)^2+(Z23-$Z$30)^2+(AA23-$AA$30)^2+(AB23-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>13364.575310716949</v>
       </c>
       <c r="AD23" s="10">
-        <f>1-(AC23/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.3890939657937722</v>
       </c>
       <c r="AE23" s="7" t="str">
-        <f>A23</f>
+        <f t="shared" si="2"/>
         <v>Rumunia</v>
       </c>
       <c r="AF23" s="11">
-        <f>AD23</f>
+        <f t="shared" si="3"/>
         <v>0.3890939657937722</v>
       </c>
       <c r="AG23" s="7" t="s">
@@ -62026,19 +62034,19 @@
         <v>144.01113543840199</v>
       </c>
       <c r="AC24" s="10">
-        <f>((B24-$B$30)^2+(C24-$C$30)^2+(D24-$D$30)^2+(E24-$E$30)^2+(F24-$F$30)^2+(G24-$G$30)^2+(H24-$H$30)^2+(I24-$I$30)^2+(J24-$J$30)^2+(K24-$K$30)^2+(L24-$L$30)^2+(M24-$M$30)^2+(N24-$N$30)^2+(O24-$O$30)^2+(P24-$P$30)^2+(Q24-$Q$30)^2+(R24-$R$30)^2+(S24-$S$30)^2+(T24-$T$30)^2+(U24-$U$30)^2+(V24-$V$30)^2+(W24-$W$30)^2+(X24-$X$30)^2+(Y24-$Y$30)^2+(Z24-$Z$30)^2+(AA24-$AA$30)^2+(AB24-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>17946.408263039437</v>
       </c>
       <c r="AD24" s="10">
-        <f>1-(AC24/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.17965450863016208</v>
       </c>
       <c r="AE24" s="7" t="str">
-        <f>A24</f>
+        <f t="shared" si="2"/>
         <v>Słowacja</v>
       </c>
       <c r="AF24" s="11">
-        <f>AD24</f>
+        <f t="shared" si="3"/>
         <v>0.17965450863016208</v>
       </c>
       <c r="AG24" s="7" t="s">
@@ -62165,19 +62173,19 @@
         <v>23.7</v>
       </c>
       <c r="AC25" s="10">
-        <f>((B25-$B$30)^2+(C25-$C$30)^2+(D25-$D$30)^2+(E25-$E$30)^2+(F25-$F$30)^2+(G25-$G$30)^2+(H25-$H$30)^2+(I25-$I$30)^2+(J25-$J$30)^2+(K25-$K$30)^2+(L25-$L$30)^2+(M25-$M$30)^2+(N25-$N$30)^2+(O25-$O$30)^2+(P25-$P$30)^2+(Q25-$Q$30)^2+(R25-$R$30)^2+(S25-$S$30)^2+(T25-$T$30)^2+(U25-$U$30)^2+(V25-$V$30)^2+(W25-$W$30)^2+(X25-$X$30)^2+(Y25-$Y$30)^2+(Z25-$Z$30)^2+(AA25-$AA$30)^2+(AB25-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>18298.541451996251</v>
       </c>
       <c r="AD25" s="10">
-        <f>1-(AC25/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.16355820291324974</v>
       </c>
       <c r="AE25" s="7" t="str">
-        <f>A25</f>
+        <f t="shared" si="2"/>
         <v>Słowenia</v>
       </c>
       <c r="AF25" s="11">
-        <f>AD25</f>
+        <f t="shared" si="3"/>
         <v>0.16355820291324974</v>
       </c>
       <c r="AG25" s="7" t="s">
@@ -62304,19 +62312,19 @@
         <v>71.900000000000006</v>
       </c>
       <c r="AC26" s="10">
-        <f>((B26-$B$30)^2+(C26-$C$30)^2+(D26-$D$30)^2+(E26-$E$30)^2+(F26-$F$30)^2+(G26-$G$30)^2+(H26-$H$30)^2+(I26-$I$30)^2+(J26-$J$30)^2+(K26-$K$30)^2+(L26-$L$30)^2+(M26-$M$30)^2+(N26-$N$30)^2+(O26-$O$30)^2+(P26-$P$30)^2+(Q26-$Q$30)^2+(R26-$R$30)^2+(S26-$S$30)^2+(T26-$T$30)^2+(U26-$U$30)^2+(V26-$V$30)^2+(W26-$W$30)^2+(X26-$X$30)^2+(Y26-$Y$30)^2+(Z26-$Z$30)^2+(AA26-$AA$30)^2+(AB26-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>14848.96036956544</v>
       </c>
       <c r="AD26" s="10">
-        <f>1-(AC26/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.32124147003889858</v>
       </c>
       <c r="AE26" s="7" t="str">
-        <f>A26</f>
+        <f t="shared" si="2"/>
         <v>Szwecja</v>
       </c>
       <c r="AF26" s="11">
-        <f>AD26</f>
+        <f t="shared" si="3"/>
         <v>0.32124147003889858</v>
       </c>
       <c r="AG26" s="7" t="s">
@@ -62443,19 +62451,19 @@
         <v>144.12425003756678</v>
       </c>
       <c r="AC27" s="10">
-        <f>((B27-$B$30)^2+(C27-$C$30)^2+(D27-$D$30)^2+(E27-$E$30)^2+(F27-$F$30)^2+(G27-$G$30)^2+(H27-$H$30)^2+(I27-$I$30)^2+(J27-$J$30)^2+(K27-$K$30)^2+(L27-$L$30)^2+(M27-$M$30)^2+(N27-$N$30)^2+(O27-$O$30)^2+(P27-$P$30)^2+(Q27-$Q$30)^2+(R27-$R$30)^2+(S27-$S$30)^2+(T27-$T$30)^2+(U27-$U$30)^2+(V27-$V$30)^2+(W27-$W$30)^2+(X27-$X$30)^2+(Y27-$Y$30)^2+(Z27-$Z$30)^2+(AA27-$AA$30)^2+(AB27-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>17953.788416067287</v>
       </c>
       <c r="AD27" s="10">
-        <f>1-(AC27/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.17931715559699357</v>
       </c>
       <c r="AE27" s="7" t="str">
-        <f>A27</f>
+        <f t="shared" si="2"/>
         <v>Węgry</v>
       </c>
       <c r="AF27" s="11">
-        <f>AD27</f>
+        <f t="shared" si="3"/>
         <v>0.17931715559699357</v>
       </c>
       <c r="AG27" s="7" t="s">
@@ -62582,19 +62590,19 @@
         <v>325.20000000000005</v>
       </c>
       <c r="AC28" s="10">
-        <f>((B28-$B$30)^2+(C28-$C$30)^2+(D28-$D$30)^2+(E28-$E$30)^2+(F28-$F$30)^2+(G28-$G$30)^2+(H28-$H$30)^2+(I28-$I$30)^2+(J28-$J$30)^2+(K28-$K$30)^2+(L28-$L$30)^2+(M28-$M$30)^2+(N28-$N$30)^2+(O28-$O$30)^2+(P28-$P$30)^2+(Q28-$Q$30)^2+(R28-$R$30)^2+(S28-$S$30)^2+(T28-$T$30)^2+(U28-$U$30)^2+(V28-$V$30)^2+(W28-$W$30)^2+(X28-$X$30)^2+(Y28-$Y$30)^2+(Z28-$Z$30)^2+(AA28-$AA$30)^2+(AB28-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>13210.248852837374</v>
       </c>
       <c r="AD28" s="10">
-        <f>1-(AC28/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.39614835863188236</v>
       </c>
       <c r="AE28" s="7" t="str">
-        <f>A28</f>
+        <f t="shared" si="2"/>
         <v>Wielka Brytania</v>
       </c>
       <c r="AF28" s="11">
-        <f>AD28</f>
+        <f t="shared" si="3"/>
         <v>0.39614835863188236</v>
       </c>
       <c r="AG28" s="7" t="s">
@@ -62721,19 +62729,19 @@
         <v>144.2523062613476</v>
       </c>
       <c r="AC29" s="10">
-        <f>((B29-$B$30)^2+(C29-$C$30)^2+(D29-$D$30)^2+(E29-$E$30)^2+(F29-$F$30)^2+(G29-$G$30)^2+(H29-$H$30)^2+(I29-$I$30)^2+(J29-$J$30)^2+(K29-$K$30)^2+(L29-$L$30)^2+(M29-$M$30)^2+(N29-$N$30)^2+(O29-$O$30)^2+(P29-$P$30)^2+(Q29-$Q$30)^2+(R29-$R$30)^2+(S29-$S$30)^2+(T29-$T$30)^2+(U29-$U$30)^2+(V29-$V$30)^2+(W29-$W$30)^2+(X29-$X$30)^2+(Y29-$Y$30)^2+(Z29-$Z$30)^2+(AA29-$AA$30)^2+(AB29-$AB$30)^2)^(0.5)</f>
+        <f t="shared" si="0"/>
         <v>14362.267977859008</v>
       </c>
       <c r="AD29" s="10">
-        <f>1-(AC29/$AI$2)</f>
+        <f t="shared" si="1"/>
         <v>0.34348859065314652</v>
       </c>
       <c r="AE29" s="7" t="str">
-        <f>A29</f>
+        <f t="shared" si="2"/>
         <v>Włochy</v>
       </c>
       <c r="AF29" s="11">
-        <f>AD29</f>
+        <f t="shared" si="3"/>
         <v>0.34348859065314652</v>
       </c>
       <c r="AG29" s="7" t="s">
@@ -62755,19 +62763,19 @@
         <v>19</v>
       </c>
       <c r="C30" s="9">
-        <f t="shared" ref="C30:F30" si="0">MAX(C29:C29)</f>
+        <f t="shared" ref="C30:F30" si="4">MAX(C29:C29)</f>
         <v>32.700000000000003</v>
       </c>
       <c r="D30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4705.63</v>
       </c>
       <c r="E30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.8</v>
       </c>
       <c r="F30" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>202</v>
       </c>
       <c r="G30" s="26">
@@ -62775,75 +62783,75 @@
         <v>61.7</v>
       </c>
       <c r="H30" s="26">
-        <f t="shared" ref="H30:P30" si="1">MIN(H2:H29)</f>
+        <f t="shared" ref="H30:P30" si="5">MIN(H2:H29)</f>
         <v>0</v>
       </c>
       <c r="I30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-5.6</v>
       </c>
       <c r="J30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>83.5</v>
       </c>
       <c r="K30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.8</v>
       </c>
       <c r="L30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.8</v>
       </c>
       <c r="M30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.4</v>
       </c>
       <c r="N30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.1</v>
       </c>
       <c r="O30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-6</v>
       </c>
       <c r="P30" s="26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>261</v>
       </c>
       <c r="Q30" s="9">
-        <f t="shared" ref="Q30:Y30" si="2">MAX(Q2:Q29)</f>
+        <f t="shared" ref="Q30:Y30" si="6">MAX(Q2:Q29)</f>
         <v>48.8</v>
       </c>
       <c r="R30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>212.6</v>
       </c>
       <c r="S30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18.62</v>
       </c>
       <c r="T30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>18560</v>
       </c>
       <c r="U30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.83</v>
       </c>
       <c r="V30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.0199999999999996</v>
       </c>
       <c r="W30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>134</v>
       </c>
       <c r="X30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>84.73</v>
       </c>
       <c r="Y30" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.4</v>
       </c>
       <c r="Z30" s="26">

</xml_diff>